<commit_message>
[commonRefush] [protocol] BagUserItemData 类修改isNew 字段 为itemNew 防止编译不通过
</commit_message>
<xml_diff>
--- a/commonRefush/src/main/resources/excel/ItemBaseCsvResource.xlsx
+++ b/commonRefush/src/main/resources/excel/ItemBaseCsvResource.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>des</t>
+  </si>
+  <si>
+    <t>quality</t>
   </si>
   <si>
     <t>int</t>
@@ -73,11 +76,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
+      <sz val="10"/>
+      <color rgb="FF9876AA"/>
+      <name val="Arial Unicode MS"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -529,7 +531,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -538,10 +540,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -550,7 +552,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -559,13 +561,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -674,11 +676,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1029,15 +1034,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L$1:L$1048576"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="7"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1059,31 +1064,37 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1105,16 +1116,19 @@
       <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -1126,7 +1140,10 @@
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>